<commit_message>
update NPCSpawner with to NPC
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/NPCPoolsData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/NPCPoolsData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>CharacterName</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>VillagerStats</t>
+  </si>
+  <si>
+    <t>VillagerB</t>
+  </si>
+  <si>
+    <t>Assets/Prefabs/NPC/VillagerB.prefab</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
         <v>50.0</v>
       </c>
       <c r="G4" s="1">
-        <v>2.0</v>
+        <v>1.5</v>
       </c>
       <c r="H4" s="1">
         <v>1.0</v>
@@ -468,15 +474,33 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1"/>

</xml_diff>

<commit_message>
update NPCStats length with devil over maxlength will dead
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/NPCPoolsData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/NPCPoolsData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>CharacterName</t>
   </si>
@@ -82,16 +82,19 @@
     <t>VillagerA</t>
   </si>
   <si>
+    <t>Assets/Prefabs/NPC/VillagerA.prefab</t>
+  </si>
+  <si>
+    <t>VillagerStats</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
     <t>Assets/Prefabs/NPC/Warrior.prefab</t>
   </si>
   <si>
-    <t>VillagerStats</t>
-  </si>
-  <si>
-    <t>VillagerB</t>
-  </si>
-  <si>
-    <t>Assets/Prefabs/NPC/VillagerB.prefab</t>
+    <t>WarriorStats</t>
   </si>
 </sst>
 </file>
@@ -458,13 +461,13 @@
         <v>24</v>
       </c>
       <c r="E4" s="1">
-        <v>30.0</v>
+        <v>10.0</v>
       </c>
       <c r="F4" s="1">
         <v>50.0</v>
       </c>
       <c r="G4" s="1">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
       <c r="H4" s="1">
         <v>1.0</v>
@@ -478,19 +481,19 @@
         <v>25</v>
       </c>
       <c r="B5" s="1">
-        <v>100.0</v>
+        <v>20.0</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
-        <v>40.0</v>
+        <v>200.0</v>
       </c>
       <c r="F5" s="1">
-        <v>40.0</v>
+        <v>100.0</v>
       </c>
       <c r="G5" s="1">
         <v>1.0</v>
@@ -557,17 +560,6 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
     <row r="12">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>

</xml_diff>